<commit_message>
Adding scripts to convert temperature netcdf
</commit_message>
<xml_diff>
--- a/docs/covariate_table.xlsx
+++ b/docs/covariate_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="460" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Covariate</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Temperature</t>
-  </si>
-  <si>
-    <t>NOAA weather stations</t>
   </si>
   <si>
     <t>McClure et al. 2015</t>
@@ -99,10 +96,6 @@
   </si>
   <si>
     <t>swine.vet.uga.edu/.nfsms/index.jsp</t>
-  </si>
-  <si>
-    <t>Ryan Miller has code that can extract temperature covariates at specific times
-so we can include a time-varying temperature layer on pig movement.</t>
   </si>
   <si>
     <t>Ryan Miller/McClure et al. 2015</t>
@@ -185,9 +178,6 @@
     <t xml:space="preserve">These will be hard masting trees only.  </t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
     <t>Cell-level</t>
   </si>
   <si>
@@ -235,6 +225,28 @@
   </si>
   <si>
     <t xml:space="preserve">Breaking it out by birds that compete for the same resources as pigs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using 0.5 degree by 0.5 degree temperature projections (50 km x 50 kmish cells).
+Temperature will vary monthly and interact with local-level variables such that the
+the local-level variable's effects on movement can vary with temperature. </t>
+  </si>
+  <si>
+    <t>NOAA data
+https://www.esrl.noaa.gov/psd/data/gridded/data.ghcncams.html</t>
+  </si>
+  <si>
+    <t>Time-varying, but constant at the 
+study level.</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Level/Dynamics</t>
+  </si>
+  <si>
+    <t>Cell-level/Varies monthly</t>
   </si>
 </sst>
 </file>
@@ -561,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,13 +596,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.2">
@@ -601,56 +613,56 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58" customHeight="1" x14ac:dyDescent="0.2">
@@ -658,164 +670,174 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
+      <c r="B8" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="92" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="92" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>60</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C18" t="s">
         <v>12</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added description for data extraction
</commit_message>
<xml_diff>
--- a/docs/covariate_table.xlsx
+++ b/docs/covariate_table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mqwilber/Dropbox/Projects/RSF_feralswine/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mqwilber/Repos/rsf_swine/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="4940" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -945,10 +945,10 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>